<commit_message>
Adds a new type (Food Form)
</commit_message>
<xml_diff>
--- a/scripts/translate/JSON_Translations.xlsx
+++ b/scripts/translate/JSON_Translations.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1390" uniqueCount="1267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1635" uniqueCount="1378">
   <si>
     <t>Identifier</t>
   </si>
@@ -1831,6 +1831,18 @@
     <t>Значение должно быть в формате час:минута</t>
   </si>
   <si>
+    <t>error.must.be.greater.than.from</t>
+  </si>
+  <si>
+    <t>Până la trebuie să fie mai mare decât De la</t>
+  </si>
+  <si>
+    <t>Until value must be greater than From</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>error.must.be.date</t>
   </si>
   <si>
@@ -3256,6 +3268,269 @@
     <t>Для настройки сторонних файлов cookie и получения дополнительной информации о конфиденциальности онлайн-рекламы IAB Romania предлагает следующий веб-сайт:</t>
   </si>
   <si>
+    <t>terms-and-conditions.title</t>
+  </si>
+  <si>
+    <t>Termeni și condiții de utilizare</t>
+  </si>
+  <si>
+    <t>terms-and-conditions.p1</t>
+  </si>
+  <si>
+    <t>Termenii și Condițiile generale de utilizare stabilesc termenii și condițiile generale de utilizare a site-ului sprijindeurgenta.ro de către potențialii vizitatori sau beneficiari.</t>
+  </si>
+  <si>
+    <t>terms-and-conditions.p2</t>
+  </si>
+  <si>
+    <t>Platforma sprijindeurgenta.ro este dezvoltată de Asociația Code for Romania (denumită în continuare “Code for Romania”) în parteneriat cu Departamentul pentru Situații de Urgență.</t>
+  </si>
+  <si>
+    <t>terms-and-conditions.p3</t>
+  </si>
+  <si>
+    <t>“sprijindeurgenta.ro” (în continuare denumit „Site”, „Platformă”, ”sprijindeurgenta.ro”) este o platformă digitală completă prin care persoanele juridice (companii, organizații neguvernamentale, autorități locale), dar și persoane fizice pot pune la dispoziție resurse pentru a veni în sprijinul persoanelor care fug din calea războiului din Ucraina. Sistemul este parte din ecosistemul național oficial de management al resurselor în situații de urgență dezvoltat de Code for Romania și administrat de Departamentul pentru Situații de Urgență.</t>
+  </si>
+  <si>
+    <t>terms-and-conditions.p4.header</t>
+  </si>
+  <si>
+    <t>1. Obiectivul Platformei</t>
+  </si>
+  <si>
+    <t>terms-and-conditions.p4.content.p1</t>
+  </si>
+  <si>
+    <t>Obiectivul sprijindeurgenta.ro este de a oferi un canal digital prin care prin care persoanele juridice (companii, organizații neguvernamentale, autorități locale), dar și persoane fizice pot pune la dispoziție resurse pentru a veni în sprijinul persoanelor care fug din calea războiului din Ucraina. Sistemul este parte din ecosistemul național oficial de management al resurselor în situații de urgență dezvoltat de Code for Romania și administrat de Departamentul pentru Situații de Urgență.</t>
+  </si>
+  <si>
+    <t>terms-and-conditions.p4.content.p2</t>
+  </si>
+  <si>
+    <t>Site-ul permite înregistrarea entităților care vor să pună la dispoziție resurse cu titlu gratuit pentru a ajuta în criza umanitară cauzată de conflictul din Ucraina. Prin formularele puse la dispoziție în platforma sprijindeurgenta.ro entitatile vor completa informatii cu privire la produsele, resursele, serviciile si expertiza voluntara pe care o pot pune la dispozitie pentru a sprijini eforturile de asistare a refugiaților care se adăpostesc în România în această perioadă de conflict.</t>
+  </si>
+  <si>
+    <t>terms-and-conditions.p4.content.p3</t>
+  </si>
+  <si>
+    <t>Persoanele fizice care doresc, de asemenea, să contribuie cu resurse vor fi direcționați către centrele de colectare organizate de organizații neguvernamentale sau de autorități publice în localitățile din țară.</t>
+  </si>
+  <si>
+    <t>terms-and-conditions.p5.header</t>
+  </si>
+  <si>
+    <t>2. Datele personale prelucrate</t>
+  </si>
+  <si>
+    <t>terms-and-conditions.p5.content</t>
+  </si>
+  <si>
+    <t>Completând formularele puse la dispoziție în paginile platformei putem colecta următoarele date:</t>
+  </si>
+  <si>
+    <t>terms-and-conditions.p5.content.li1</t>
+  </si>
+  <si>
+    <t>Denumirea entității publice sau private</t>
+  </si>
+  <si>
+    <t>terms-and-conditions.p5.content.li2</t>
+  </si>
+  <si>
+    <t>Adresa de e-mail a entității publice sau private</t>
+  </si>
+  <si>
+    <t>terms-and-conditions.p5.content.li3</t>
+  </si>
+  <si>
+    <t>Numărul de telefon al entității publice sau private</t>
+  </si>
+  <si>
+    <t>terms-and-conditions.p6.header</t>
+  </si>
+  <si>
+    <t>3. Scop și temei</t>
+  </si>
+  <si>
+    <t>terms-and-conditions.p6.content</t>
+  </si>
+  <si>
+    <t>Code for Romania prelucrează datele entităților persoane juridice, publice sau private, doar în scopul de a crea acestora un cont de utilizator în care pot adăuga, edita sau șterge resurse pe care doresc să le pună la dispoziție pentru a fi utilizate cu scopul de a sprijini persoanele vulnerabile care acum se refugiază din Ucraina pe teritoriul României.</t>
+  </si>
+  <si>
+    <t>terms-and-conditions.p7.header</t>
+  </si>
+  <si>
+    <t>4. Durata stocării</t>
+  </si>
+  <si>
+    <t>terms-and-conditions.p7.content</t>
+  </si>
+  <si>
+    <t>Datele furnizate sunt stocate temporar pe durata funcționării platformei sprijindeurgenta.ro în contextul crizei umanitare cauzate de conflictul armat din Ucraina.</t>
+  </si>
+  <si>
+    <t>terms-and-conditions.p8.header</t>
+  </si>
+  <si>
+    <t>5. Transmiterea datelor către terți</t>
+  </si>
+  <si>
+    <t>terms-and-conditions.p8.content</t>
+  </si>
+  <si>
+    <t>Datele furnizate sunt utilizate de către Centrul Național de Coordonare și Comandă a Intervenției și structurile sale teritoriale pentru a putea coordona intervenția în cadrul acestei situații de urgență. Datele pot fi transmise către alte instituții sau autorități publice, precum și alte organe abilitate ale statului, în baza și în limitele prevederilor legale, ca urmare a unor cereri expres formulate de acestea.</t>
+  </si>
+  <si>
+    <t>terms-and-conditions.p9.header</t>
+  </si>
+  <si>
+    <t>6. Drepturile tale</t>
+  </si>
+  <si>
+    <t>terms-and-conditions.p9.content</t>
+  </si>
+  <si>
+    <t>În calitate de utilizator al platformei sprijindeurgenta.ro, potrivit Legii nr. 679/2016, precum și, începând cu 25 mai 2018, potrivit Regulamentului General privind protecția datelor, ai următoarele drepturi:</t>
+  </si>
+  <si>
+    <t>terms-and-conditions.p9.content.li1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dreptul la informare cu privire la prelucrarea datelor;
+</t>
+  </si>
+  <si>
+    <t>terms-and-conditions.p9.content.li2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dreptul de acces la datele furnizate, la cerere și în mod gratuit pentru o solicitare pe an;
+</t>
+  </si>
+  <si>
+    <t>terms-and-conditions.p9.content.li3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dreptul de intervenție, rectificarea, ștergerea sau portabilitatea datelor, la cerere și în mod gratuit;
+</t>
+  </si>
+  <si>
+    <t>terms-and-conditions.p9.content.li4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dreptul de a te adresa Autorității Naționale de Supraveghere privind Prelucrarea Datelor cu Caracter Personal (cu sediul în Bucureşti, sector 1, B-dul G-ral. Gheorghe Magheru, www.dataprotection.ro) sau justiției, pentru apărarea oricăror drepturi garantate de lege;
+</t>
+  </si>
+  <si>
+    <t>terms-and-conditions.p9.content.li5</t>
+  </si>
+  <si>
+    <t>Dreptul la opoziţie şi procesul decizional individual automatizat;</t>
+  </si>
+  <si>
+    <t>terms-and-conditions.p9.content.li6</t>
+  </si>
+  <si>
+    <t>începând cu 25 mai 2018, potrivit Regulamentului general privind protecția datelor, dreptul la restricționarea prelucrării.</t>
+  </si>
+  <si>
+    <t>terms-and-conditions.p10.header</t>
+  </si>
+  <si>
+    <t>7. Securitate și confidențialitate</t>
+  </si>
+  <si>
+    <t>terms-and-conditions.p10.content.p1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protecția informațiilor în cursul prelucrării datelor colectate este o preocupare majoră a Code for Romania, de aceea toate datele colectate în cursul vizitelor pe sprijindeurgenta.ro sunt prelucrate conform prevederilor legale în vigoare în România. Code for Romania folosește tehnologii de ultimă generație și ia toate măsurile tehnice rezonabile pentru transmiterea și păstrarea datelor în condiții de deplină securitate și confidențialitate.
+</t>
+  </si>
+  <si>
+    <t>terms-and-conditions.p10.content.p2</t>
+  </si>
+  <si>
+    <t>Toate datele de pe site sunt stocate și procesate pe servere situate în Uniunea Europeană, ce cad sub incidența legislației europene de protecție a datelor personale. Nicio informație oferită pe acest site nu părăsește teritoriul Uniunii Europene.</t>
+  </si>
+  <si>
+    <t>terms-and-conditions.p10.content.p3</t>
+  </si>
+  <si>
+    <t>Dacă descoperim un incident cu privire la securitatea datelor care prezintă un risc pentru drepturile și libertățile utilizatorilor noștri, vom notifica Autoritatea Națională de Supraveghere privind Prelucrarea Datelor cu Caracter Personale în termen de 72 de ore. Dacă incidentul de securitate este de natură să prezinte un risc ridicat pentru drepturile și libertățile tale, vei fi, de asemenea, notificat.</t>
+  </si>
+  <si>
+    <t>terms-and-conditions.p10.content.p4</t>
+  </si>
+  <si>
+    <t>Este strict interzisă folosirea acestui Site în scopul distrugerii sau alterării lui, a conținutului său a securității acestuia ori pentru discreditarea sau hărțuirea sprijindeurgenta.ro sau a Code for Romania.</t>
+  </si>
+  <si>
+    <t>terms-and-conditions.p10.content.p5</t>
+  </si>
+  <si>
+    <t>Code for Romania va aplica toate măsurile de securitate tehnică și organizatorică pentru protejarea datelor asupra cărora deține controlul împotriva oricărei situații de manipulare accidentală sau intenționată, pierdere, distrugere sau împotriva accesului unei persoane neautorizate.</t>
+  </si>
+  <si>
+    <t>terms-and-conditions.p11.header</t>
+  </si>
+  <si>
+    <t>8. Modificari Termeni și Condiții generale de utilizare Site</t>
+  </si>
+  <si>
+    <t>terms-and-conditions.p11.content.p1</t>
+  </si>
+  <si>
+    <t>"Termenii și Condițiile generale de utilizare" constituie, în întregime, un acord încheiat între dumneavoastră și Code for Romania în privința utilizării sprijindeurgenta.ro.</t>
+  </si>
+  <si>
+    <t>terms-and-conditions.p11.content.p2</t>
+  </si>
+  <si>
+    <t>Code for Romania își rezervă dreptul de a revizui și aduce la zi "Termenii și Condițiile generale de utilizare" în orice moment, fără o anunțare sau o acceptare prealabilă a utilizatorilor.</t>
+  </si>
+  <si>
+    <t>terms-and-conditions.p11.content.p3</t>
+  </si>
+  <si>
+    <t>Dacă aveți întrebări cu privire la informațiile cuprinse în această pagină vă rugăm să ne scrieți la adresa dopomoha@code4.ro.</t>
+  </si>
+  <si>
+    <t>terms-and-conditions.p12.header</t>
+  </si>
+  <si>
+    <t>9. Despre Code for Romania</t>
+  </si>
+  <si>
+    <t>terms-and-conditions.p12.content</t>
+  </si>
+  <si>
+    <t>Code for Romania este o organizație neguvernamentală independentă, neafiliată politic și apolitică, înființată în anul 2016, al cărei scop este de a mobiliza tinerii profesioniști din domeniul IT să creeze instrumente digitale care ajută în soluționarea problemelor sociale. Code for Romania este înființată și funcționează în conformitate cu legea română, actul constitutiv și statutul său și codul de conduită.</t>
+  </si>
+  <si>
+    <t>terms-and-conditions.p13.header</t>
+  </si>
+  <si>
+    <t>10. Contactează Code for Romania</t>
+  </si>
+  <si>
+    <t>terms-and-conditions.p13.content.p1</t>
+  </si>
+  <si>
+    <t>Pentru orice întrebări sau preocupări, precum și pentru exercitarea drepturilor tale legate de prelucrarea datelor de către Code for Romania, ne poti contacta la:</t>
+  </si>
+  <si>
+    <t>terms-and-conditions.p13.content.p2</t>
+  </si>
+  <si>
+    <t>Adresa: Piața Alba Iulia nr. 7, bloc I6, etaj 1, ap. 6, mun. București, Romania</t>
+  </si>
+  <si>
+    <t>terms-and-conditions.p13.content.p3</t>
+  </si>
+  <si>
+    <t>E-mail: contact@code4.ro</t>
+  </si>
+  <si>
     <t>error.availability.required</t>
   </si>
   <si>
@@ -3811,7 +4086,70 @@
     <t>Правительство</t>
   </si>
   <si>
-    <t/>
+    <t>Translator/Traducător</t>
+  </si>
+  <si>
+    <t>Translator</t>
+  </si>
+  <si>
+    <t>Перекладач</t>
+  </si>
+  <si>
+    <t>Переводчик</t>
+  </si>
+  <si>
+    <t>Veterinar</t>
+  </si>
+  <si>
+    <t>Veterinarian</t>
+  </si>
+  <si>
+    <t>Ветеринар</t>
+  </si>
+  <si>
+    <t>signup.products.sanitary.materials</t>
+  </si>
+  <si>
+    <t>Materiale sanitare</t>
+  </si>
+  <si>
+    <t>Sanitary materials</t>
+  </si>
+  <si>
+    <t>Матеріали першої допомоги</t>
+  </si>
+  <si>
+    <t>Материалы первой помощи</t>
+  </si>
+  <si>
+    <t>signup.products.medicine</t>
+  </si>
+  <si>
+    <t>Medicamente</t>
+  </si>
+  <si>
+    <t>Medicine</t>
+  </si>
+  <si>
+    <t>Ліки</t>
+  </si>
+  <si>
+    <t>Медикаменты</t>
+  </si>
+  <si>
+    <t>foodform</t>
+  </si>
+  <si>
+    <t>Pentru organizațiile și autoritățile care gestionează centre de refugiați: pentru a solicita necesarul de porții zilnice de alimente de care aveți nevoie în centru, apăsați aici.</t>
+  </si>
+  <si>
+    <t>If you are an organization or authority that manages refugee centers and want to request the daily food rations you need, click here.</t>
+  </si>
+  <si>
+    <t>Для організацій та органів влади, які керують центрами для біженців: Щоб запитати щоденні харчові пайки, які вам потрібні в центрі, натисніть тут.</t>
+  </si>
+  <si>
+    <t>Для организаций и органов, управляющих центрами для беженцев: Чтобы запросить дневной рацион питания, который вам нужен в центре, нажмите здесь.</t>
   </si>
 </sst>
 </file>
@@ -4188,7 +4526,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E278"/>
+  <dimension ref="A1:E327"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -6381,41 +6719,41 @@
         <v>609</v>
       </c>
       <c r="E129" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
+        <v>610</v>
+      </c>
+      <c r="B130" t="s">
         <v>611</v>
       </c>
-      <c r="B130" t="s">
-        <v>123</v>
-      </c>
       <c r="C130" t="s">
-        <v>124</v>
+        <v>612</v>
       </c>
       <c r="D130" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="E130" t="s">
-        <v>126</v>
+        <v>614</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
       <c r="B131" t="s">
-        <v>614</v>
+        <v>123</v>
       </c>
       <c r="C131" t="s">
-        <v>615</v>
+        <v>124</v>
       </c>
       <c r="D131" t="s">
-        <v>125</v>
+        <v>616</v>
       </c>
       <c r="E131" t="s">
-        <v>616</v>
+        <v>126</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
@@ -6429,92 +6767,92 @@
         <v>619</v>
       </c>
       <c r="D132" t="s">
+        <v>125</v>
+      </c>
+      <c r="E132" t="s">
         <v>620</v>
-      </c>
-      <c r="E132" t="s">
-        <v>621</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
+        <v>621</v>
+      </c>
+      <c r="B133" t="s">
         <v>622</v>
       </c>
-      <c r="B133" t="s">
+      <c r="C133" t="s">
         <v>623</v>
       </c>
-      <c r="C133" t="s">
+      <c r="D133" t="s">
         <v>624</v>
       </c>
-      <c r="D133" t="s">
+      <c r="E133" t="s">
         <v>625</v>
-      </c>
-      <c r="E133" t="s">
-        <v>626</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
+        <v>626</v>
+      </c>
+      <c r="B134" t="s">
         <v>627</v>
       </c>
-      <c r="B134" t="s">
+      <c r="C134" t="s">
         <v>628</v>
       </c>
-      <c r="C134" t="s">
+      <c r="D134" t="s">
         <v>629</v>
       </c>
-      <c r="D134" t="s">
+      <c r="E134" t="s">
         <v>630</v>
-      </c>
-      <c r="E134" t="s">
-        <v>631</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
+        <v>631</v>
+      </c>
+      <c r="B135" t="s">
         <v>632</v>
       </c>
-      <c r="B135" t="s">
+      <c r="C135" t="s">
         <v>633</v>
       </c>
-      <c r="C135" t="s">
+      <c r="D135" t="s">
         <v>634</v>
       </c>
-      <c r="D135" t="s">
+      <c r="E135" t="s">
         <v>635</v>
-      </c>
-      <c r="E135" t="s">
-        <v>636</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
+        <v>636</v>
+      </c>
+      <c r="B136" t="s">
         <v>637</v>
       </c>
-      <c r="B136" t="s">
+      <c r="C136" t="s">
         <v>638</v>
       </c>
-      <c r="C136" t="s">
+      <c r="D136" t="s">
         <v>639</v>
       </c>
-      <c r="D136" t="s">
+      <c r="E136" t="s">
         <v>640</v>
-      </c>
-      <c r="E136" t="s">
-        <v>641</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
+        <v>641</v>
+      </c>
+      <c r="B137" t="s">
         <v>642</v>
       </c>
-      <c r="B137" t="s">
+      <c r="C137" t="s">
         <v>643</v>
       </c>
-      <c r="C137" t="s">
+      <c r="D137" t="s">
         <v>644</v>
-      </c>
-      <c r="D137" t="s">
-        <v>645</v>
       </c>
       <c r="E137" t="s">
         <v>645</v>
@@ -6534,21 +6872,21 @@
         <v>649</v>
       </c>
       <c r="E138" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
+        <v>650</v>
+      </c>
+      <c r="B139" t="s">
         <v>651</v>
       </c>
-      <c r="B139" t="s">
+      <c r="C139" t="s">
         <v>652</v>
       </c>
-      <c r="C139" t="s">
+      <c r="D139" t="s">
         <v>653</v>
-      </c>
-      <c r="D139" t="s">
-        <v>654</v>
       </c>
       <c r="E139" t="s">
         <v>654</v>
@@ -6568,225 +6906,225 @@
         <v>658</v>
       </c>
       <c r="E140" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
+        <v>659</v>
+      </c>
+      <c r="B141" t="s">
         <v>660</v>
       </c>
-      <c r="B141" t="s">
+      <c r="C141" t="s">
         <v>661</v>
       </c>
-      <c r="C141" t="s">
+      <c r="D141" t="s">
         <v>662</v>
       </c>
-      <c r="D141" t="s">
+      <c r="E141" t="s">
         <v>663</v>
-      </c>
-      <c r="E141" t="s">
-        <v>664</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
+        <v>664</v>
+      </c>
+      <c r="B142" t="s">
         <v>665</v>
       </c>
-      <c r="B142" t="s">
+      <c r="C142" t="s">
         <v>666</v>
-      </c>
-      <c r="C142" t="s">
-        <v>593</v>
       </c>
       <c r="D142" t="s">
         <v>667</v>
       </c>
       <c r="E142" t="s">
-        <v>595</v>
+        <v>668</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="B143" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="C143" t="s">
-        <v>670</v>
+        <v>593</v>
       </c>
       <c r="D143" t="s">
         <v>671</v>
       </c>
       <c r="E143" t="s">
-        <v>672</v>
+        <v>595</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
+        <v>672</v>
+      </c>
+      <c r="B144" t="s">
         <v>673</v>
       </c>
-      <c r="B144" t="s">
+      <c r="C144" t="s">
         <v>674</v>
       </c>
-      <c r="C144" t="s">
-        <v>670</v>
-      </c>
       <c r="D144" t="s">
-        <v>671</v>
+        <v>675</v>
       </c>
       <c r="E144" t="s">
-        <v>672</v>
+        <v>676</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
+        <v>677</v>
+      </c>
+      <c r="B145" t="s">
+        <v>678</v>
+      </c>
+      <c r="C145" t="s">
+        <v>674</v>
+      </c>
+      <c r="D145" t="s">
         <v>675</v>
       </c>
-      <c r="B145" t="s">
+      <c r="E145" t="s">
         <v>676</v>
-      </c>
-      <c r="C145" t="s">
-        <v>677</v>
-      </c>
-      <c r="D145" t="s">
-        <v>678</v>
-      </c>
-      <c r="E145" t="s">
-        <v>679</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
+        <v>679</v>
+      </c>
+      <c r="B146" t="s">
         <v>680</v>
       </c>
-      <c r="B146" t="s">
+      <c r="C146" t="s">
         <v>681</v>
       </c>
-      <c r="C146" t="s">
+      <c r="D146" t="s">
         <v>682</v>
       </c>
-      <c r="D146" t="s">
+      <c r="E146" t="s">
         <v>683</v>
-      </c>
-      <c r="E146" t="s">
-        <v>684</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
+        <v>684</v>
+      </c>
+      <c r="B147" t="s">
         <v>685</v>
       </c>
-      <c r="B147" t="s">
+      <c r="C147" t="s">
         <v>686</v>
       </c>
-      <c r="C147" t="s">
+      <c r="D147" t="s">
         <v>687</v>
       </c>
-      <c r="D147" t="s">
+      <c r="E147" t="s">
         <v>688</v>
-      </c>
-      <c r="E147" t="s">
-        <v>689</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
+        <v>689</v>
+      </c>
+      <c r="B148" t="s">
         <v>690</v>
       </c>
-      <c r="B148" t="s">
+      <c r="C148" t="s">
         <v>691</v>
       </c>
-      <c r="C148" t="s">
+      <c r="D148" t="s">
         <v>692</v>
       </c>
-      <c r="D148" t="s">
+      <c r="E148" t="s">
         <v>693</v>
-      </c>
-      <c r="E148" t="s">
-        <v>694</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
+        <v>694</v>
+      </c>
+      <c r="B149" t="s">
         <v>695</v>
       </c>
-      <c r="B149" t="s">
+      <c r="C149" t="s">
         <v>696</v>
       </c>
-      <c r="C149" t="s">
+      <c r="D149" t="s">
         <v>697</v>
       </c>
-      <c r="D149" t="s">
+      <c r="E149" t="s">
         <v>698</v>
-      </c>
-      <c r="E149" t="s">
-        <v>699</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
+        <v>699</v>
+      </c>
+      <c r="B150" t="s">
         <v>700</v>
       </c>
-      <c r="B150" t="s">
+      <c r="C150" t="s">
         <v>701</v>
       </c>
-      <c r="C150" t="s">
+      <c r="D150" t="s">
         <v>702</v>
       </c>
-      <c r="D150" t="s">
+      <c r="E150" t="s">
         <v>703</v>
-      </c>
-      <c r="E150" t="s">
-        <v>704</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
+        <v>704</v>
+      </c>
+      <c r="B151" t="s">
         <v>705</v>
       </c>
-      <c r="B151" t="s">
+      <c r="C151" t="s">
         <v>706</v>
       </c>
-      <c r="C151" t="s">
+      <c r="D151" t="s">
         <v>707</v>
       </c>
-      <c r="D151" t="s">
+      <c r="E151" t="s">
         <v>708</v>
-      </c>
-      <c r="E151" t="s">
-        <v>709</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
+        <v>709</v>
+      </c>
+      <c r="B152" t="s">
         <v>710</v>
       </c>
-      <c r="B152" t="s">
+      <c r="C152" t="s">
         <v>711</v>
       </c>
-      <c r="C152" t="s">
+      <c r="D152" t="s">
         <v>712</v>
       </c>
-      <c r="D152" t="s">
+      <c r="E152" t="s">
         <v>713</v>
-      </c>
-      <c r="E152" t="s">
-        <v>714</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
+        <v>714</v>
+      </c>
+      <c r="B153" t="s">
         <v>715</v>
       </c>
-      <c r="B153" t="s">
+      <c r="C153" t="s">
         <v>716</v>
       </c>
-      <c r="C153" t="s">
+      <c r="D153" t="s">
         <v>717</v>
-      </c>
-      <c r="D153" t="s">
-        <v>135</v>
       </c>
       <c r="E153" t="s">
         <v>718</v>
@@ -6797,840 +7135,840 @@
         <v>719</v>
       </c>
       <c r="B154" t="s">
-        <v>497</v>
+        <v>720</v>
       </c>
       <c r="C154" t="s">
-        <v>498</v>
+        <v>721</v>
       </c>
       <c r="D154" t="s">
-        <v>720</v>
+        <v>135</v>
       </c>
       <c r="E154" t="s">
-        <v>500</v>
+        <v>722</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>721</v>
+        <v>723</v>
       </c>
       <c r="B155" t="s">
-        <v>482</v>
+        <v>497</v>
       </c>
       <c r="C155" t="s">
-        <v>483</v>
+        <v>498</v>
       </c>
       <c r="D155" t="s">
-        <v>722</v>
+        <v>724</v>
       </c>
       <c r="E155" t="s">
-        <v>723</v>
+        <v>500</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="B156" t="s">
-        <v>725</v>
+        <v>482</v>
       </c>
       <c r="C156" t="s">
+        <v>483</v>
+      </c>
+      <c r="D156" t="s">
         <v>726</v>
       </c>
-      <c r="D156" t="s">
+      <c r="E156" t="s">
         <v>727</v>
-      </c>
-      <c r="E156" t="s">
-        <v>728</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
+        <v>728</v>
+      </c>
+      <c r="B157" t="s">
         <v>729</v>
       </c>
-      <c r="B157" t="s">
-        <v>293</v>
-      </c>
       <c r="C157" t="s">
-        <v>294</v>
+        <v>730</v>
       </c>
       <c r="D157" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="E157" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="B158" t="s">
-        <v>733</v>
+        <v>293</v>
       </c>
       <c r="C158" t="s">
+        <v>294</v>
+      </c>
+      <c r="D158" t="s">
         <v>734</v>
       </c>
-      <c r="D158" t="s">
+      <c r="E158" t="s">
         <v>735</v>
-      </c>
-      <c r="E158" t="s">
-        <v>736</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
+        <v>736</v>
+      </c>
+      <c r="B159" t="s">
         <v>737</v>
       </c>
-      <c r="B159" t="s">
+      <c r="C159" t="s">
         <v>738</v>
       </c>
-      <c r="C159" t="s">
+      <c r="D159" t="s">
         <v>739</v>
       </c>
-      <c r="D159" t="s">
+      <c r="E159" t="s">
         <v>740</v>
-      </c>
-      <c r="E159" t="s">
-        <v>741</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
+        <v>741</v>
+      </c>
+      <c r="B160" t="s">
         <v>742</v>
       </c>
-      <c r="B160" t="s">
+      <c r="C160" t="s">
         <v>743</v>
       </c>
-      <c r="C160" t="s">
+      <c r="D160" t="s">
         <v>744</v>
       </c>
-      <c r="D160" t="s">
+      <c r="E160" t="s">
         <v>745</v>
-      </c>
-      <c r="E160" t="s">
-        <v>746</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
+        <v>746</v>
+      </c>
+      <c r="B161" t="s">
         <v>747</v>
       </c>
-      <c r="B161" t="s">
+      <c r="C161" t="s">
         <v>748</v>
       </c>
-      <c r="C161" t="s">
+      <c r="D161" t="s">
         <v>749</v>
       </c>
-      <c r="D161" t="s">
+      <c r="E161" t="s">
         <v>750</v>
-      </c>
-      <c r="E161" t="s">
-        <v>751</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
+        <v>751</v>
+      </c>
+      <c r="B162" t="s">
         <v>752</v>
       </c>
-      <c r="B162" t="s">
+      <c r="C162" t="s">
         <v>753</v>
       </c>
-      <c r="C162" t="s">
+      <c r="D162" t="s">
         <v>754</v>
       </c>
-      <c r="D162" t="s">
+      <c r="E162" t="s">
         <v>755</v>
-      </c>
-      <c r="E162" t="s">
-        <v>756</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
+        <v>756</v>
+      </c>
+      <c r="B163" t="s">
         <v>757</v>
       </c>
-      <c r="B163" t="s">
+      <c r="C163" t="s">
         <v>758</v>
       </c>
-      <c r="C163" t="s">
+      <c r="D163" t="s">
         <v>759</v>
       </c>
-      <c r="D163" t="s">
+      <c r="E163" t="s">
         <v>760</v>
-      </c>
-      <c r="E163" t="s">
-        <v>761</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
+        <v>761</v>
+      </c>
+      <c r="B164" t="s">
         <v>762</v>
       </c>
-      <c r="B164" t="s">
+      <c r="C164" t="s">
         <v>763</v>
       </c>
-      <c r="C164" t="s">
+      <c r="D164" t="s">
         <v>764</v>
       </c>
-      <c r="D164" t="s">
+      <c r="E164" t="s">
         <v>765</v>
-      </c>
-      <c r="E164" t="s">
-        <v>766</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
+        <v>766</v>
+      </c>
+      <c r="B165" t="s">
         <v>767</v>
       </c>
-      <c r="B165" t="s">
+      <c r="C165" t="s">
         <v>768</v>
       </c>
-      <c r="C165" t="s">
+      <c r="D165" t="s">
         <v>769</v>
       </c>
-      <c r="D165" t="s">
+      <c r="E165" t="s">
         <v>770</v>
-      </c>
-      <c r="E165" t="s">
-        <v>771</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
+        <v>771</v>
+      </c>
+      <c r="B166" t="s">
         <v>772</v>
       </c>
-      <c r="B166" t="s">
+      <c r="C166" t="s">
         <v>773</v>
       </c>
-      <c r="C166" t="s">
+      <c r="D166" t="s">
         <v>774</v>
       </c>
-      <c r="D166" t="s">
+      <c r="E166" t="s">
         <v>775</v>
-      </c>
-      <c r="E166" t="s">
-        <v>776</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
+        <v>776</v>
+      </c>
+      <c r="B167" t="s">
         <v>777</v>
       </c>
-      <c r="B167" t="s">
+      <c r="C167" t="s">
         <v>778</v>
       </c>
-      <c r="C167" t="s">
+      <c r="D167" t="s">
         <v>779</v>
       </c>
-      <c r="D167" t="s">
+      <c r="E167" t="s">
         <v>780</v>
-      </c>
-      <c r="E167" t="s">
-        <v>781</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
+        <v>781</v>
+      </c>
+      <c r="B168" t="s">
         <v>782</v>
       </c>
-      <c r="B168" t="s">
+      <c r="C168" t="s">
         <v>783</v>
       </c>
-      <c r="C168" t="s">
+      <c r="D168" t="s">
         <v>784</v>
       </c>
-      <c r="D168" t="s">
+      <c r="E168" t="s">
         <v>785</v>
-      </c>
-      <c r="E168" t="s">
-        <v>786</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
+        <v>786</v>
+      </c>
+      <c r="B169" t="s">
         <v>787</v>
       </c>
-      <c r="B169" t="s">
+      <c r="C169" t="s">
         <v>788</v>
       </c>
-      <c r="C169" t="s">
+      <c r="D169" t="s">
         <v>789</v>
       </c>
-      <c r="D169" t="s">
+      <c r="E169" t="s">
         <v>790</v>
-      </c>
-      <c r="E169" t="s">
-        <v>791</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
+        <v>791</v>
+      </c>
+      <c r="B170" t="s">
         <v>792</v>
       </c>
-      <c r="B170" t="s">
+      <c r="C170" t="s">
         <v>793</v>
       </c>
-      <c r="C170" t="s">
+      <c r="D170" t="s">
         <v>794</v>
       </c>
-      <c r="D170" t="s">
+      <c r="E170" t="s">
         <v>795</v>
-      </c>
-      <c r="E170" t="s">
-        <v>796</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
+        <v>796</v>
+      </c>
+      <c r="B171" t="s">
         <v>797</v>
       </c>
-      <c r="B171" t="s">
+      <c r="C171" t="s">
         <v>798</v>
       </c>
-      <c r="C171" t="s">
+      <c r="D171" t="s">
         <v>799</v>
       </c>
-      <c r="D171" t="s">
+      <c r="E171" t="s">
         <v>800</v>
-      </c>
-      <c r="E171" t="s">
-        <v>801</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
+        <v>801</v>
+      </c>
+      <c r="B172" t="s">
         <v>802</v>
       </c>
-      <c r="B172" t="s">
+      <c r="C172" t="s">
         <v>803</v>
-      </c>
-      <c r="C172" t="s">
-        <v>759</v>
       </c>
       <c r="D172" t="s">
         <v>804</v>
       </c>
       <c r="E172" t="s">
-        <v>761</v>
+        <v>805</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="B173" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="C173" t="s">
-        <v>807</v>
+        <v>763</v>
       </c>
       <c r="D173" t="s">
         <v>808</v>
       </c>
       <c r="E173" t="s">
-        <v>809</v>
+        <v>765</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
+        <v>809</v>
+      </c>
+      <c r="B174" t="s">
         <v>810</v>
       </c>
-      <c r="B174" t="s">
+      <c r="C174" t="s">
         <v>811</v>
       </c>
-      <c r="C174" t="s">
+      <c r="D174" t="s">
         <v>812</v>
       </c>
-      <c r="D174" t="s">
+      <c r="E174" t="s">
         <v>813</v>
-      </c>
-      <c r="E174" t="s">
-        <v>814</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
+        <v>814</v>
+      </c>
+      <c r="B175" t="s">
         <v>815</v>
       </c>
-      <c r="B175" t="s">
+      <c r="C175" t="s">
         <v>816</v>
       </c>
-      <c r="C175" t="s">
+      <c r="D175" t="s">
         <v>817</v>
       </c>
-      <c r="D175" t="s">
+      <c r="E175" t="s">
         <v>818</v>
-      </c>
-      <c r="E175" t="s">
-        <v>819</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
+        <v>819</v>
+      </c>
+      <c r="B176" t="s">
         <v>820</v>
       </c>
-      <c r="B176" t="s">
+      <c r="C176" t="s">
         <v>821</v>
       </c>
-      <c r="C176" t="s">
-        <v>417</v>
-      </c>
       <c r="D176" t="s">
-        <v>418</v>
+        <v>822</v>
       </c>
       <c r="E176" t="s">
-        <v>419</v>
+        <v>823</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
       <c r="B177" t="s">
-        <v>823</v>
+        <v>825</v>
       </c>
       <c r="C177" t="s">
-        <v>824</v>
+        <v>417</v>
       </c>
       <c r="D177" t="s">
-        <v>825</v>
+        <v>418</v>
       </c>
       <c r="E177" t="s">
-        <v>826</v>
+        <v>419</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
+        <v>826</v>
+      </c>
+      <c r="B178" t="s">
         <v>827</v>
       </c>
-      <c r="B178" t="s">
+      <c r="C178" t="s">
         <v>828</v>
       </c>
-      <c r="C178" t="s">
+      <c r="D178" t="s">
         <v>829</v>
       </c>
-      <c r="D178" t="s">
+      <c r="E178" t="s">
         <v>830</v>
-      </c>
-      <c r="E178" t="s">
-        <v>831</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
+        <v>831</v>
+      </c>
+      <c r="B179" t="s">
         <v>832</v>
       </c>
-      <c r="B179" t="s">
+      <c r="C179" t="s">
         <v>833</v>
       </c>
-      <c r="C179" t="s">
+      <c r="D179" t="s">
         <v>834</v>
       </c>
-      <c r="D179" t="s">
+      <c r="E179" t="s">
         <v>835</v>
-      </c>
-      <c r="E179" t="s">
-        <v>836</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
+        <v>836</v>
+      </c>
+      <c r="B180" t="s">
         <v>837</v>
       </c>
-      <c r="B180" t="s">
+      <c r="C180" t="s">
         <v>838</v>
       </c>
-      <c r="C180" t="s">
+      <c r="D180" t="s">
         <v>839</v>
       </c>
-      <c r="D180" t="s">
+      <c r="E180" t="s">
         <v>840</v>
-      </c>
-      <c r="E180" t="s">
-        <v>841</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
+        <v>841</v>
+      </c>
+      <c r="B181" t="s">
         <v>842</v>
       </c>
-      <c r="B181" t="s">
+      <c r="C181" t="s">
         <v>843</v>
       </c>
-      <c r="C181" t="s">
+      <c r="D181" t="s">
         <v>844</v>
       </c>
-      <c r="D181" t="s">
+      <c r="E181" t="s">
         <v>845</v>
-      </c>
-      <c r="E181" t="s">
-        <v>846</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
+        <v>846</v>
+      </c>
+      <c r="B182" t="s">
         <v>847</v>
       </c>
-      <c r="B182" t="s">
+      <c r="C182" t="s">
         <v>848</v>
       </c>
-      <c r="C182" t="s">
+      <c r="D182" t="s">
         <v>849</v>
       </c>
-      <c r="D182" t="s">
+      <c r="E182" t="s">
         <v>850</v>
-      </c>
-      <c r="E182" t="s">
-        <v>851</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
+        <v>851</v>
+      </c>
+      <c r="B183" t="s">
         <v>852</v>
       </c>
-      <c r="B183" t="s">
+      <c r="C183" t="s">
         <v>853</v>
       </c>
-      <c r="C183" t="s">
+      <c r="D183" t="s">
         <v>854</v>
       </c>
-      <c r="D183" t="s">
+      <c r="E183" t="s">
         <v>855</v>
-      </c>
-      <c r="E183" t="s">
-        <v>856</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
+        <v>856</v>
+      </c>
+      <c r="B184" t="s">
         <v>857</v>
       </c>
-      <c r="B184" t="s">
+      <c r="C184" t="s">
         <v>858</v>
       </c>
-      <c r="C184" t="s">
+      <c r="D184" t="s">
         <v>859</v>
       </c>
-      <c r="D184" t="s">
+      <c r="E184" t="s">
         <v>860</v>
-      </c>
-      <c r="E184" t="s">
-        <v>861</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
+        <v>861</v>
+      </c>
+      <c r="B185" t="s">
         <v>862</v>
       </c>
-      <c r="B185" t="s">
+      <c r="C185" t="s">
         <v>863</v>
       </c>
-      <c r="C185" t="s">
+      <c r="D185" t="s">
         <v>864</v>
       </c>
-      <c r="D185" t="s">
+      <c r="E185" t="s">
         <v>865</v>
-      </c>
-      <c r="E185" t="s">
-        <v>866</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
+        <v>866</v>
+      </c>
+      <c r="B186" t="s">
         <v>867</v>
       </c>
-      <c r="B186" t="s">
+      <c r="C186" t="s">
         <v>868</v>
       </c>
-      <c r="C186" t="s">
+      <c r="D186" t="s">
         <v>869</v>
       </c>
-      <c r="D186" t="s">
+      <c r="E186" t="s">
         <v>870</v>
-      </c>
-      <c r="E186" t="s">
-        <v>871</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
+        <v>871</v>
+      </c>
+      <c r="B187" t="s">
         <v>872</v>
       </c>
-      <c r="B187" t="s">
+      <c r="C187" t="s">
         <v>873</v>
       </c>
-      <c r="C187" t="s">
+      <c r="D187" t="s">
         <v>874</v>
       </c>
-      <c r="D187" t="s">
+      <c r="E187" t="s">
         <v>875</v>
-      </c>
-      <c r="E187" t="s">
-        <v>876</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
+        <v>876</v>
+      </c>
+      <c r="B188" t="s">
         <v>877</v>
       </c>
-      <c r="B188" t="s">
+      <c r="C188" t="s">
         <v>878</v>
       </c>
-      <c r="C188" t="s">
+      <c r="D188" t="s">
         <v>879</v>
       </c>
-      <c r="D188" t="s">
+      <c r="E188" t="s">
         <v>880</v>
-      </c>
-      <c r="E188" t="s">
-        <v>881</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
+        <v>881</v>
+      </c>
+      <c r="B189" t="s">
         <v>882</v>
       </c>
-      <c r="B189" t="s">
+      <c r="C189" t="s">
         <v>883</v>
       </c>
-      <c r="C189" t="s">
+      <c r="D189" t="s">
         <v>884</v>
       </c>
-      <c r="D189" t="s">
+      <c r="E189" t="s">
         <v>885</v>
-      </c>
-      <c r="E189" t="s">
-        <v>886</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
+        <v>886</v>
+      </c>
+      <c r="B190" t="s">
         <v>887</v>
       </c>
-      <c r="B190" t="s">
+      <c r="C190" t="s">
         <v>888</v>
       </c>
-      <c r="C190" t="s">
+      <c r="D190" t="s">
         <v>889</v>
       </c>
-      <c r="D190" t="s">
+      <c r="E190" t="s">
         <v>890</v>
-      </c>
-      <c r="E190" t="s">
-        <v>891</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
+        <v>891</v>
+      </c>
+      <c r="B191" t="s">
         <v>892</v>
       </c>
-      <c r="B191" t="s">
+      <c r="C191" t="s">
         <v>893</v>
       </c>
-      <c r="C191" t="s">
+      <c r="D191" t="s">
         <v>894</v>
       </c>
-      <c r="D191" t="s">
+      <c r="E191" t="s">
         <v>895</v>
-      </c>
-      <c r="E191" t="s">
-        <v>896</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
+        <v>896</v>
+      </c>
+      <c r="B192" t="s">
         <v>897</v>
       </c>
-      <c r="B192" t="s">
+      <c r="C192" t="s">
         <v>898</v>
       </c>
-      <c r="C192" t="s">
+      <c r="D192" t="s">
         <v>899</v>
       </c>
-      <c r="D192" t="s">
+      <c r="E192" t="s">
         <v>900</v>
-      </c>
-      <c r="E192" t="s">
-        <v>901</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
+        <v>901</v>
+      </c>
+      <c r="B193" t="s">
         <v>902</v>
       </c>
-      <c r="B193" t="s">
+      <c r="C193" t="s">
         <v>903</v>
       </c>
-      <c r="C193" t="s">
+      <c r="D193" t="s">
         <v>904</v>
       </c>
-      <c r="D193" t="s">
+      <c r="E193" t="s">
         <v>905</v>
-      </c>
-      <c r="E193" t="s">
-        <v>906</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
+        <v>906</v>
+      </c>
+      <c r="B194" t="s">
         <v>907</v>
       </c>
-      <c r="B194" t="s">
+      <c r="C194" t="s">
         <v>908</v>
       </c>
-      <c r="C194" t="s">
+      <c r="D194" t="s">
         <v>909</v>
       </c>
-      <c r="D194" t="s">
+      <c r="E194" t="s">
         <v>910</v>
-      </c>
-      <c r="E194" t="s">
-        <v>911</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
+        <v>911</v>
+      </c>
+      <c r="B195" t="s">
         <v>912</v>
       </c>
-      <c r="B195" t="s">
+      <c r="C195" t="s">
         <v>913</v>
       </c>
-      <c r="C195" t="s">
+      <c r="D195" t="s">
         <v>914</v>
       </c>
-      <c r="D195" t="s">
+      <c r="E195" t="s">
         <v>915</v>
-      </c>
-      <c r="E195" t="s">
-        <v>916</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
+        <v>916</v>
+      </c>
+      <c r="B196" t="s">
         <v>917</v>
       </c>
-      <c r="B196" t="s">
+      <c r="C196" t="s">
         <v>918</v>
       </c>
-      <c r="C196" t="s">
+      <c r="D196" t="s">
         <v>919</v>
       </c>
-      <c r="D196" t="s">
+      <c r="E196" t="s">
         <v>920</v>
-      </c>
-      <c r="E196" t="s">
-        <v>921</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
+        <v>921</v>
+      </c>
+      <c r="B197" t="s">
         <v>922</v>
       </c>
-      <c r="B197" t="s">
+      <c r="C197" t="s">
         <v>923</v>
       </c>
-      <c r="C197" t="s">
+      <c r="D197" t="s">
         <v>924</v>
       </c>
-      <c r="D197" t="s">
+      <c r="E197" t="s">
         <v>925</v>
-      </c>
-      <c r="E197" t="s">
-        <v>926</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
+        <v>926</v>
+      </c>
+      <c r="B198" t="s">
         <v>927</v>
       </c>
-      <c r="B198" t="s">
+      <c r="C198" t="s">
         <v>928</v>
       </c>
-      <c r="C198" t="s">
+      <c r="D198" t="s">
         <v>929</v>
       </c>
-      <c r="D198" t="s">
+      <c r="E198" t="s">
         <v>930</v>
-      </c>
-      <c r="E198" t="s">
-        <v>931</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
+        <v>931</v>
+      </c>
+      <c r="B199" t="s">
         <v>932</v>
       </c>
-      <c r="B199" t="s">
+      <c r="C199" t="s">
         <v>933</v>
       </c>
-      <c r="C199" t="s">
+      <c r="D199" t="s">
         <v>934</v>
       </c>
-      <c r="D199" t="s">
+      <c r="E199" t="s">
         <v>935</v>
-      </c>
-      <c r="E199" t="s">
-        <v>936</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
+        <v>936</v>
+      </c>
+      <c r="B200" t="s">
         <v>937</v>
       </c>
-      <c r="B200" t="s">
+      <c r="C200" t="s">
         <v>938</v>
       </c>
-      <c r="C200" t="s">
+      <c r="D200" t="s">
         <v>939</v>
       </c>
-      <c r="D200" t="s">
+      <c r="E200" t="s">
         <v>940</v>
-      </c>
-      <c r="E200" t="s">
-        <v>941</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
+        <v>941</v>
+      </c>
+      <c r="B201" t="s">
         <v>942</v>
       </c>
-      <c r="B201" t="s">
+      <c r="C201" t="s">
         <v>943</v>
       </c>
-      <c r="C201" t="s">
+      <c r="D201" t="s">
         <v>944</v>
       </c>
-      <c r="D201" t="s">
+      <c r="E201" t="s">
         <v>945</v>
-      </c>
-      <c r="E201" t="s">
-        <v>946</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
+        <v>946</v>
+      </c>
+      <c r="B202" t="s">
         <v>947</v>
       </c>
-      <c r="B202" t="s">
+      <c r="C202" t="s">
         <v>948</v>
       </c>
-      <c r="C202" t="s">
+      <c r="D202" t="s">
         <v>949</v>
       </c>
-      <c r="D202" t="s">
+      <c r="E202" t="s">
         <v>950</v>
-      </c>
-      <c r="E202" t="s">
-        <v>951</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
+        <v>951</v>
+      </c>
+      <c r="B203" t="s">
         <v>952</v>
-      </c>
-      <c r="B203" t="s">
-        <v>953</v>
       </c>
       <c r="C203" t="s">
         <v>953</v>
@@ -7650,1271 +7988,2104 @@
         <v>957</v>
       </c>
       <c r="C204" t="s">
+        <v>957</v>
+      </c>
+      <c r="D204" t="s">
         <v>958</v>
       </c>
-      <c r="D204" t="s">
+      <c r="E204" t="s">
         <v>959</v>
-      </c>
-      <c r="E204" t="s">
-        <v>960</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
+        <v>960</v>
+      </c>
+      <c r="B205" t="s">
         <v>961</v>
       </c>
-      <c r="B205" t="s">
+      <c r="C205" t="s">
         <v>962</v>
       </c>
-      <c r="C205" t="s">
+      <c r="D205" t="s">
         <v>963</v>
       </c>
-      <c r="D205" t="s">
+      <c r="E205" t="s">
         <v>964</v>
-      </c>
-      <c r="E205" t="s">
-        <v>965</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
+        <v>965</v>
+      </c>
+      <c r="B206" t="s">
         <v>966</v>
       </c>
-      <c r="B206" t="s">
+      <c r="C206" t="s">
         <v>967</v>
       </c>
-      <c r="C206" t="s">
+      <c r="D206" t="s">
         <v>968</v>
       </c>
-      <c r="D206" t="s">
+      <c r="E206" t="s">
         <v>969</v>
-      </c>
-      <c r="E206" t="s">
-        <v>970</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
+        <v>970</v>
+      </c>
+      <c r="B207" t="s">
         <v>971</v>
       </c>
-      <c r="B207" t="s">
+      <c r="C207" t="s">
         <v>972</v>
       </c>
-      <c r="C207" t="s">
+      <c r="D207" t="s">
         <v>973</v>
       </c>
-      <c r="D207" t="s">
+      <c r="E207" t="s">
         <v>974</v>
-      </c>
-      <c r="E207" t="s">
-        <v>975</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
+        <v>975</v>
+      </c>
+      <c r="B208" t="s">
         <v>976</v>
       </c>
-      <c r="B208" t="s">
+      <c r="C208" t="s">
         <v>977</v>
       </c>
-      <c r="C208" t="s">
+      <c r="D208" t="s">
         <v>978</v>
       </c>
-      <c r="D208" t="s">
+      <c r="E208" t="s">
         <v>979</v>
-      </c>
-      <c r="E208" t="s">
-        <v>980</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
+        <v>980</v>
+      </c>
+      <c r="B209" t="s">
         <v>981</v>
       </c>
-      <c r="B209" t="s">
+      <c r="C209" t="s">
         <v>982</v>
       </c>
-      <c r="C209" t="s">
+      <c r="D209" t="s">
         <v>983</v>
       </c>
-      <c r="D209" t="s">
+      <c r="E209" t="s">
         <v>984</v>
-      </c>
-      <c r="E209" t="s">
-        <v>985</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
+        <v>985</v>
+      </c>
+      <c r="B210" t="s">
         <v>986</v>
       </c>
-      <c r="B210" t="s">
+      <c r="C210" t="s">
         <v>987</v>
       </c>
-      <c r="C210" t="s">
+      <c r="D210" t="s">
         <v>988</v>
       </c>
-      <c r="D210" t="s">
+      <c r="E210" t="s">
         <v>989</v>
-      </c>
-      <c r="E210" t="s">
-        <v>990</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
+        <v>990</v>
+      </c>
+      <c r="B211" t="s">
         <v>991</v>
       </c>
-      <c r="B211" t="s">
+      <c r="C211" t="s">
         <v>992</v>
       </c>
-      <c r="C211" t="s">
+      <c r="D211" t="s">
         <v>993</v>
       </c>
-      <c r="D211" t="s">
+      <c r="E211" t="s">
         <v>994</v>
-      </c>
-      <c r="E211" t="s">
-        <v>995</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
+        <v>995</v>
+      </c>
+      <c r="B212" t="s">
         <v>996</v>
       </c>
-      <c r="B212" t="s">
+      <c r="C212" t="s">
         <v>997</v>
       </c>
-      <c r="C212" t="s">
+      <c r="D212" t="s">
         <v>998</v>
       </c>
-      <c r="D212" t="s">
+      <c r="E212" t="s">
         <v>999</v>
-      </c>
-      <c r="E212" t="s">
-        <v>1000</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
+        <v>1000</v>
+      </c>
+      <c r="B213" t="s">
         <v>1001</v>
       </c>
-      <c r="B213" t="s">
+      <c r="C213" t="s">
         <v>1002</v>
       </c>
-      <c r="C213" t="s">
+      <c r="D213" t="s">
         <v>1003</v>
       </c>
-      <c r="D213" t="s">
+      <c r="E213" t="s">
         <v>1004</v>
-      </c>
-      <c r="E213" t="s">
-        <v>1005</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
+        <v>1005</v>
+      </c>
+      <c r="B214" t="s">
         <v>1006</v>
       </c>
-      <c r="B214" t="s">
+      <c r="C214" t="s">
         <v>1007</v>
       </c>
-      <c r="C214" t="s">
+      <c r="D214" t="s">
         <v>1008</v>
       </c>
-      <c r="D214" t="s">
+      <c r="E214" t="s">
         <v>1009</v>
-      </c>
-      <c r="E214" t="s">
-        <v>1010</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
+        <v>1010</v>
+      </c>
+      <c r="B215" t="s">
         <v>1011</v>
       </c>
-      <c r="B215" t="s">
+      <c r="C215" t="s">
         <v>1012</v>
       </c>
-      <c r="C215" t="s">
+      <c r="D215" t="s">
         <v>1013</v>
       </c>
-      <c r="D215" t="s">
+      <c r="E215" t="s">
         <v>1014</v>
-      </c>
-      <c r="E215" t="s">
-        <v>1015</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B216" t="s">
         <v>1016</v>
       </c>
-      <c r="B216" t="s">
+      <c r="C216" t="s">
         <v>1017</v>
       </c>
-      <c r="C216" t="s">
+      <c r="D216" t="s">
         <v>1018</v>
       </c>
-      <c r="D216" t="s">
+      <c r="E216" t="s">
         <v>1019</v>
-      </c>
-      <c r="E216" t="s">
-        <v>1020</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B217" t="s">
         <v>1021</v>
       </c>
-      <c r="B217" t="s">
+      <c r="C217" t="s">
         <v>1022</v>
       </c>
-      <c r="C217" t="s">
+      <c r="D217" t="s">
         <v>1023</v>
       </c>
-      <c r="D217" t="s">
+      <c r="E217" t="s">
         <v>1024</v>
-      </c>
-      <c r="E217" t="s">
-        <v>1025</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
+        <v>1025</v>
+      </c>
+      <c r="B218" t="s">
         <v>1026</v>
       </c>
-      <c r="B218" t="s">
+      <c r="C218" t="s">
         <v>1027</v>
       </c>
-      <c r="C218" t="s">
+      <c r="D218" t="s">
         <v>1028</v>
       </c>
-      <c r="D218" t="s">
+      <c r="E218" t="s">
         <v>1029</v>
-      </c>
-      <c r="E218" t="s">
-        <v>1030</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
+        <v>1030</v>
+      </c>
+      <c r="B219" t="s">
         <v>1031</v>
       </c>
-      <c r="B219" t="s">
+      <c r="C219" t="s">
         <v>1032</v>
       </c>
-      <c r="C219" t="s">
+      <c r="D219" t="s">
         <v>1033</v>
       </c>
-      <c r="D219" t="s">
+      <c r="E219" t="s">
         <v>1034</v>
-      </c>
-      <c r="E219" t="s">
-        <v>1035</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B220" t="s">
         <v>1036</v>
       </c>
-      <c r="B220" t="s">
+      <c r="C220" t="s">
         <v>1037</v>
       </c>
-      <c r="C220" t="s">
+      <c r="D220" t="s">
         <v>1038</v>
       </c>
-      <c r="D220" t="s">
+      <c r="E220" t="s">
         <v>1039</v>
-      </c>
-      <c r="E220" t="s">
-        <v>1040</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B221" t="s">
         <v>1041</v>
       </c>
-      <c r="B221" t="s">
+      <c r="C221" t="s">
         <v>1042</v>
       </c>
-      <c r="C221" t="s">
+      <c r="D221" t="s">
         <v>1043</v>
       </c>
-      <c r="D221" t="s">
+      <c r="E221" t="s">
         <v>1044</v>
-      </c>
-      <c r="E221" t="s">
-        <v>1045</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
+        <v>1045</v>
+      </c>
+      <c r="B222" t="s">
         <v>1046</v>
       </c>
-      <c r="B222" t="s">
+      <c r="C222" t="s">
         <v>1047</v>
       </c>
-      <c r="C222" t="s">
+      <c r="D222" t="s">
         <v>1048</v>
       </c>
-      <c r="D222" t="s">
+      <c r="E222" t="s">
         <v>1049</v>
-      </c>
-      <c r="E222" t="s">
-        <v>1050</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B223" t="s">
         <v>1051</v>
       </c>
-      <c r="B223" t="s">
+      <c r="C223" t="s">
         <v>1052</v>
       </c>
-      <c r="C223" t="s">
+      <c r="D223" t="s">
         <v>1053</v>
       </c>
-      <c r="D223" t="s">
+      <c r="E223" t="s">
         <v>1054</v>
-      </c>
-      <c r="E223" t="s">
-        <v>1055</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B224" t="s">
         <v>1056</v>
       </c>
-      <c r="B224" t="s">
+      <c r="C224" t="s">
         <v>1057</v>
       </c>
-      <c r="C224" t="s">
+      <c r="D224" t="s">
         <v>1058</v>
       </c>
-      <c r="D224" t="s">
+      <c r="E224" t="s">
         <v>1059</v>
-      </c>
-      <c r="E224" t="s">
-        <v>1060</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B225" t="s">
         <v>1061</v>
       </c>
-      <c r="B225" t="s">
+      <c r="C225" t="s">
         <v>1062</v>
       </c>
-      <c r="C225" t="s">
+      <c r="D225" t="s">
         <v>1063</v>
       </c>
-      <c r="D225" t="s">
+      <c r="E225" t="s">
         <v>1064</v>
-      </c>
-      <c r="E225" t="s">
-        <v>1065</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B226" t="s">
         <v>1066</v>
       </c>
-      <c r="B226" t="s">
+      <c r="C226" t="s">
         <v>1067</v>
       </c>
-      <c r="C226" t="s">
+      <c r="D226" t="s">
         <v>1068</v>
       </c>
-      <c r="D226" t="s">
+      <c r="E226" t="s">
         <v>1069</v>
-      </c>
-      <c r="E226" t="s">
-        <v>1070</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
+        <v>1070</v>
+      </c>
+      <c r="B227" t="s">
         <v>1071</v>
       </c>
-      <c r="B227" t="s">
+      <c r="C227" t="s">
         <v>1072</v>
       </c>
-      <c r="C227" t="s">
+      <c r="D227" t="s">
         <v>1073</v>
       </c>
-      <c r="D227" t="s">
+      <c r="E227" t="s">
         <v>1074</v>
-      </c>
-      <c r="E227" t="s">
-        <v>1075</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
+        <v>1075</v>
+      </c>
+      <c r="B228" t="s">
         <v>1076</v>
       </c>
-      <c r="B228" t="s">
+      <c r="C228" t="s">
         <v>1077</v>
       </c>
-      <c r="C228" t="s">
+      <c r="D228" t="s">
         <v>1078</v>
       </c>
-      <c r="D228" t="s">
+      <c r="E228" t="s">
         <v>1079</v>
-      </c>
-      <c r="E228" t="s">
-        <v>1080</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B229" t="s">
         <v>1081</v>
       </c>
-      <c r="B229" t="s">
+      <c r="C229" t="s">
         <v>1082</v>
       </c>
-      <c r="C229" t="s">
+      <c r="D229" t="s">
         <v>1083</v>
       </c>
-      <c r="D229" t="s">
+      <c r="E229" t="s">
         <v>1084</v>
-      </c>
-      <c r="E229" t="s">
-        <v>1085</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
+        <v>1085</v>
+      </c>
+      <c r="B230" t="s">
         <v>1086</v>
       </c>
-      <c r="B230" t="s">
-        <v>1087</v>
-      </c>
       <c r="C230" t="s">
-        <v>1088</v>
+        <v>609</v>
       </c>
       <c r="D230" t="s">
-        <v>1089</v>
+        <v>609</v>
       </c>
       <c r="E230" t="s">
-        <v>1089</v>
+        <v>609</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>1090</v>
+        <v>1087</v>
       </c>
       <c r="B231" t="s">
-        <v>1091</v>
+        <v>1088</v>
       </c>
       <c r="C231" t="s">
-        <v>1092</v>
+        <v>609</v>
       </c>
       <c r="D231" t="s">
-        <v>1093</v>
+        <v>609</v>
       </c>
       <c r="E231" t="s">
-        <v>1094</v>
+        <v>609</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>1095</v>
+        <v>1089</v>
       </c>
       <c r="B232" t="s">
-        <v>138</v>
+        <v>1090</v>
       </c>
       <c r="C232" t="s">
-        <v>139</v>
+        <v>609</v>
       </c>
       <c r="D232" t="s">
-        <v>140</v>
+        <v>609</v>
       </c>
       <c r="E232" t="s">
-        <v>140</v>
+        <v>609</v>
       </c>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>1096</v>
+        <v>1091</v>
       </c>
       <c r="B233" t="s">
-        <v>1097</v>
+        <v>1092</v>
       </c>
       <c r="C233" t="s">
-        <v>1098</v>
+        <v>609</v>
       </c>
       <c r="D233" t="s">
-        <v>1099</v>
+        <v>609</v>
       </c>
       <c r="E233" t="s">
-        <v>1100</v>
+        <v>609</v>
       </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>1101</v>
+        <v>1093</v>
       </c>
       <c r="B234" t="s">
-        <v>1102</v>
+        <v>1094</v>
       </c>
       <c r="C234" t="s">
-        <v>1103</v>
+        <v>609</v>
       </c>
       <c r="D234" t="s">
-        <v>1104</v>
+        <v>609</v>
       </c>
       <c r="E234" t="s">
-        <v>1105</v>
+        <v>609</v>
       </c>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>1106</v>
+        <v>1095</v>
       </c>
       <c r="B235" t="s">
-        <v>1107</v>
+        <v>1096</v>
       </c>
       <c r="C235" t="s">
-        <v>1108</v>
+        <v>609</v>
       </c>
       <c r="D235" t="s">
-        <v>1109</v>
+        <v>609</v>
       </c>
       <c r="E235" t="s">
-        <v>1110</v>
+        <v>609</v>
       </c>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>1111</v>
+        <v>1097</v>
       </c>
       <c r="B236" t="s">
-        <v>1112</v>
+        <v>1098</v>
       </c>
       <c r="C236" t="s">
-        <v>1113</v>
+        <v>609</v>
       </c>
       <c r="D236" t="s">
-        <v>1114</v>
+        <v>609</v>
       </c>
       <c r="E236" t="s">
-        <v>1115</v>
+        <v>609</v>
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>1116</v>
+        <v>1099</v>
       </c>
       <c r="B237" t="s">
-        <v>1117</v>
+        <v>1100</v>
       </c>
       <c r="C237" t="s">
-        <v>1118</v>
+        <v>609</v>
       </c>
       <c r="D237" t="s">
-        <v>1119</v>
+        <v>609</v>
       </c>
       <c r="E237" t="s">
-        <v>1120</v>
+        <v>609</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>1121</v>
+        <v>1101</v>
       </c>
       <c r="B238" t="s">
-        <v>1122</v>
+        <v>1102</v>
       </c>
       <c r="C238" t="s">
-        <v>1123</v>
+        <v>609</v>
       </c>
       <c r="D238" t="s">
-        <v>1124</v>
+        <v>609</v>
       </c>
       <c r="E238" t="s">
-        <v>1125</v>
+        <v>609</v>
       </c>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>1126</v>
+        <v>1103</v>
       </c>
       <c r="B239" t="s">
-        <v>1127</v>
+        <v>1104</v>
       </c>
       <c r="C239" t="s">
-        <v>1128</v>
+        <v>609</v>
       </c>
       <c r="D239" t="s">
-        <v>1129</v>
+        <v>609</v>
       </c>
       <c r="E239" t="s">
-        <v>1130</v>
+        <v>609</v>
       </c>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>1131</v>
+        <v>1105</v>
       </c>
       <c r="B240" t="s">
-        <v>1132</v>
+        <v>1106</v>
       </c>
       <c r="C240" t="s">
-        <v>1133</v>
+        <v>609</v>
       </c>
       <c r="D240" t="s">
-        <v>1134</v>
+        <v>609</v>
       </c>
       <c r="E240" t="s">
-        <v>1135</v>
+        <v>609</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>1136</v>
+        <v>1107</v>
       </c>
       <c r="B241" t="s">
-        <v>1137</v>
+        <v>1108</v>
       </c>
       <c r="C241" t="s">
-        <v>1138</v>
+        <v>609</v>
       </c>
       <c r="D241" t="s">
-        <v>1139</v>
+        <v>609</v>
       </c>
       <c r="E241" t="s">
-        <v>1140</v>
+        <v>609</v>
       </c>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>1141</v>
+        <v>1109</v>
       </c>
       <c r="B242" t="s">
-        <v>816</v>
+        <v>1110</v>
       </c>
       <c r="C242" t="s">
-        <v>1142</v>
+        <v>609</v>
       </c>
       <c r="D242" t="s">
-        <v>1143</v>
+        <v>609</v>
       </c>
       <c r="E242" t="s">
-        <v>1144</v>
+        <v>609</v>
       </c>
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>1145</v>
+        <v>1111</v>
       </c>
       <c r="B243" t="s">
-        <v>1146</v>
+        <v>1112</v>
       </c>
       <c r="C243" t="s">
-        <v>1147</v>
+        <v>609</v>
       </c>
       <c r="D243" t="s">
-        <v>1148</v>
+        <v>609</v>
       </c>
       <c r="E243" t="s">
-        <v>1149</v>
+        <v>609</v>
       </c>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>1150</v>
+        <v>1113</v>
       </c>
       <c r="B244" t="s">
-        <v>406</v>
+        <v>1114</v>
       </c>
       <c r="C244" t="s">
-        <v>388</v>
+        <v>609</v>
       </c>
       <c r="D244" t="s">
-        <v>398</v>
+        <v>609</v>
       </c>
       <c r="E244" t="s">
-        <v>399</v>
+        <v>609</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>1151</v>
+        <v>1115</v>
       </c>
       <c r="B245" t="s">
-        <v>1152</v>
+        <v>1116</v>
       </c>
       <c r="C245" t="s">
-        <v>1153</v>
+        <v>609</v>
       </c>
       <c r="D245" t="s">
-        <v>1154</v>
+        <v>609</v>
       </c>
       <c r="E245" t="s">
-        <v>1155</v>
+        <v>609</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>1156</v>
+        <v>1117</v>
       </c>
       <c r="B246" t="s">
-        <v>123</v>
+        <v>1118</v>
       </c>
       <c r="C246" t="s">
-        <v>124</v>
+        <v>609</v>
       </c>
       <c r="D246" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="E246" t="s">
-        <v>126</v>
+        <v>609</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>1157</v>
+        <v>1119</v>
       </c>
       <c r="B247" t="s">
-        <v>133</v>
+        <v>1120</v>
       </c>
       <c r="C247" t="s">
-        <v>1158</v>
+        <v>609</v>
       </c>
       <c r="D247" t="s">
-        <v>1159</v>
+        <v>609</v>
       </c>
       <c r="E247" t="s">
-        <v>1120</v>
+        <v>609</v>
       </c>
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>1160</v>
+        <v>1121</v>
       </c>
       <c r="B248" t="s">
-        <v>128</v>
+        <v>1122</v>
       </c>
       <c r="C248" t="s">
-        <v>129</v>
+        <v>609</v>
       </c>
       <c r="D248" t="s">
-        <v>1161</v>
+        <v>609</v>
       </c>
       <c r="E248" t="s">
-        <v>131</v>
+        <v>609</v>
       </c>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>1162</v>
+        <v>1123</v>
       </c>
       <c r="B249" t="s">
-        <v>138</v>
+        <v>1124</v>
       </c>
       <c r="C249" t="s">
-        <v>139</v>
+        <v>609</v>
       </c>
       <c r="D249" t="s">
-        <v>140</v>
+        <v>609</v>
       </c>
       <c r="E249" t="s">
-        <v>140</v>
+        <v>609</v>
       </c>
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>1163</v>
+        <v>1125</v>
       </c>
       <c r="B250" t="s">
-        <v>1164</v>
+        <v>1126</v>
       </c>
       <c r="C250" t="s">
-        <v>1165</v>
+        <v>609</v>
       </c>
       <c r="D250" t="s">
-        <v>1166</v>
+        <v>609</v>
       </c>
       <c r="E250" t="s">
-        <v>1167</v>
+        <v>609</v>
       </c>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>1168</v>
+        <v>1127</v>
       </c>
       <c r="B251" t="s">
-        <v>492</v>
+        <v>1128</v>
       </c>
       <c r="C251" t="s">
-        <v>493</v>
+        <v>609</v>
       </c>
       <c r="D251" t="s">
-        <v>494</v>
+        <v>609</v>
       </c>
       <c r="E251" t="s">
-        <v>495</v>
+        <v>609</v>
       </c>
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>1169</v>
+        <v>1129</v>
       </c>
       <c r="B252" t="s">
-        <v>1170</v>
+        <v>1130</v>
       </c>
       <c r="C252" t="s">
-        <v>1171</v>
+        <v>609</v>
       </c>
       <c r="D252" t="s">
-        <v>1172</v>
+        <v>609</v>
       </c>
       <c r="E252" t="s">
-        <v>1173</v>
+        <v>609</v>
       </c>
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>1174</v>
+        <v>1131</v>
       </c>
       <c r="B253" t="s">
-        <v>1175</v>
+        <v>1132</v>
       </c>
       <c r="C253" t="s">
-        <v>1176</v>
+        <v>609</v>
       </c>
       <c r="D253" t="s">
-        <v>1177</v>
+        <v>609</v>
       </c>
       <c r="E253" t="s">
-        <v>1178</v>
+        <v>609</v>
       </c>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>1179</v>
+        <v>1133</v>
       </c>
       <c r="B254" t="s">
-        <v>16</v>
+        <v>1134</v>
       </c>
       <c r="C254" t="s">
-        <v>1180</v>
+        <v>609</v>
       </c>
       <c r="D254" t="s">
-        <v>18</v>
+        <v>609</v>
       </c>
       <c r="E254" t="s">
-        <v>19</v>
+        <v>609</v>
       </c>
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>1181</v>
+        <v>1135</v>
       </c>
       <c r="B255" t="s">
-        <v>1181</v>
+        <v>1136</v>
       </c>
       <c r="C255" t="s">
-        <v>1182</v>
+        <v>609</v>
       </c>
       <c r="D255" t="s">
-        <v>1183</v>
+        <v>609</v>
       </c>
       <c r="E255" t="s">
-        <v>1184</v>
+        <v>609</v>
       </c>
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>1185</v>
+        <v>1137</v>
       </c>
       <c r="B256" t="s">
-        <v>1185</v>
+        <v>1138</v>
       </c>
       <c r="C256" t="s">
-        <v>1186</v>
+        <v>609</v>
       </c>
       <c r="D256" t="s">
-        <v>1187</v>
+        <v>609</v>
       </c>
       <c r="E256" t="s">
-        <v>1187</v>
+        <v>609</v>
       </c>
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>1188</v>
+        <v>1139</v>
       </c>
       <c r="B257" t="s">
-        <v>1188</v>
+        <v>1140</v>
       </c>
       <c r="C257" t="s">
-        <v>1189</v>
+        <v>609</v>
       </c>
       <c r="D257" t="s">
-        <v>1190</v>
+        <v>609</v>
       </c>
       <c r="E257" t="s">
-        <v>1191</v>
+        <v>609</v>
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>1192</v>
+        <v>1141</v>
       </c>
       <c r="B258" t="s">
-        <v>1192</v>
+        <v>1142</v>
       </c>
       <c r="C258" t="s">
-        <v>1193</v>
+        <v>609</v>
       </c>
       <c r="D258" t="s">
-        <v>1194</v>
+        <v>609</v>
       </c>
       <c r="E258" t="s">
-        <v>1194</v>
+        <v>609</v>
       </c>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>1195</v>
+        <v>1143</v>
       </c>
       <c r="B259" t="s">
-        <v>1195</v>
+        <v>1144</v>
       </c>
       <c r="C259" t="s">
-        <v>1196</v>
+        <v>609</v>
       </c>
       <c r="D259" t="s">
-        <v>1197</v>
+        <v>609</v>
       </c>
       <c r="E259" t="s">
-        <v>1198</v>
+        <v>609</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>133</v>
+        <v>1145</v>
       </c>
       <c r="B260" t="s">
-        <v>133</v>
+        <v>1146</v>
       </c>
       <c r="C260" t="s">
-        <v>134</v>
+        <v>609</v>
       </c>
       <c r="D260" t="s">
-        <v>1159</v>
+        <v>609</v>
       </c>
       <c r="E260" t="s">
-        <v>1199</v>
+        <v>609</v>
       </c>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>1200</v>
+        <v>1147</v>
       </c>
       <c r="B261" t="s">
-        <v>1200</v>
+        <v>1148</v>
       </c>
       <c r="C261" t="s">
-        <v>1201</v>
+        <v>609</v>
       </c>
       <c r="D261" t="s">
-        <v>1202</v>
+        <v>609</v>
       </c>
       <c r="E261" t="s">
-        <v>1202</v>
+        <v>609</v>
       </c>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>1203</v>
+        <v>1149</v>
       </c>
       <c r="B262" t="s">
-        <v>1203</v>
+        <v>1150</v>
       </c>
       <c r="C262" t="s">
-        <v>1204</v>
+        <v>609</v>
       </c>
       <c r="D262" t="s">
-        <v>1205</v>
+        <v>609</v>
       </c>
       <c r="E262" t="s">
-        <v>1206</v>
+        <v>609</v>
       </c>
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>1207</v>
+        <v>1151</v>
       </c>
       <c r="B263" t="s">
-        <v>1117</v>
+        <v>1152</v>
       </c>
       <c r="C263" t="s">
-        <v>1118</v>
+        <v>609</v>
       </c>
       <c r="D263" t="s">
-        <v>1208</v>
+        <v>609</v>
       </c>
       <c r="E263" t="s">
-        <v>1120</v>
+        <v>609</v>
       </c>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>1209</v>
+        <v>1153</v>
       </c>
       <c r="B264" t="s">
-        <v>1209</v>
+        <v>1154</v>
       </c>
       <c r="C264" t="s">
-        <v>1210</v>
+        <v>609</v>
       </c>
       <c r="D264" t="s">
-        <v>1211</v>
+        <v>609</v>
       </c>
       <c r="E264" t="s">
-        <v>1212</v>
+        <v>609</v>
       </c>
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>1213</v>
+        <v>1155</v>
       </c>
       <c r="B265" t="s">
-        <v>1213</v>
+        <v>1156</v>
       </c>
       <c r="C265" t="s">
-        <v>1214</v>
+        <v>609</v>
       </c>
       <c r="D265" t="s">
-        <v>1215</v>
+        <v>609</v>
       </c>
       <c r="E265" t="s">
-        <v>1216</v>
+        <v>609</v>
       </c>
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>1217</v>
+        <v>1157</v>
       </c>
       <c r="B266" t="s">
-        <v>1217</v>
+        <v>1158</v>
       </c>
       <c r="C266" t="s">
-        <v>1218</v>
+        <v>609</v>
       </c>
       <c r="D266" t="s">
-        <v>1219</v>
+        <v>609</v>
       </c>
       <c r="E266" t="s">
-        <v>1220</v>
+        <v>609</v>
       </c>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>1221</v>
+        <v>1159</v>
       </c>
       <c r="B267" t="s">
-        <v>1221</v>
+        <v>1160</v>
       </c>
       <c r="C267" t="s">
-        <v>1222</v>
+        <v>609</v>
       </c>
       <c r="D267" t="s">
-        <v>1223</v>
+        <v>609</v>
       </c>
       <c r="E267" t="s">
-        <v>1224</v>
+        <v>609</v>
       </c>
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>1225</v>
+        <v>1161</v>
       </c>
       <c r="B268" t="s">
-        <v>1226</v>
+        <v>1162</v>
       </c>
       <c r="C268" t="s">
-        <v>1227</v>
+        <v>609</v>
       </c>
       <c r="D268" t="s">
-        <v>1228</v>
+        <v>609</v>
       </c>
       <c r="E268" t="s">
-        <v>1229</v>
+        <v>609</v>
       </c>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>1230</v>
+        <v>1163</v>
       </c>
       <c r="B269" t="s">
-        <v>1231</v>
+        <v>1164</v>
       </c>
       <c r="C269" t="s">
-        <v>1232</v>
+        <v>609</v>
       </c>
       <c r="D269" t="s">
-        <v>1233</v>
+        <v>609</v>
       </c>
       <c r="E269" t="s">
-        <v>1234</v>
+        <v>609</v>
       </c>
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>1235</v>
+        <v>1165</v>
       </c>
       <c r="B270" t="s">
-        <v>1236</v>
+        <v>1166</v>
       </c>
       <c r="C270" t="s">
-        <v>1237</v>
+        <v>609</v>
       </c>
       <c r="D270" t="s">
-        <v>1238</v>
+        <v>609</v>
       </c>
       <c r="E270" t="s">
-        <v>1239</v>
+        <v>609</v>
       </c>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>1240</v>
+        <v>1167</v>
       </c>
       <c r="B271" t="s">
-        <v>1241</v>
+        <v>1168</v>
       </c>
       <c r="C271" t="s">
-        <v>1242</v>
+        <v>609</v>
       </c>
       <c r="D271" t="s">
-        <v>1243</v>
+        <v>609</v>
       </c>
       <c r="E271" t="s">
-        <v>1244</v>
+        <v>609</v>
       </c>
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>1245</v>
+        <v>1169</v>
       </c>
       <c r="B272" t="s">
-        <v>1246</v>
+        <v>1170</v>
       </c>
       <c r="C272" t="s">
-        <v>1247</v>
+        <v>609</v>
       </c>
       <c r="D272" t="s">
-        <v>1248</v>
+        <v>609</v>
       </c>
       <c r="E272" t="s">
-        <v>1249</v>
+        <v>609</v>
       </c>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>1250</v>
+        <v>1171</v>
       </c>
       <c r="B273" t="s">
-        <v>1251</v>
+        <v>1172</v>
       </c>
       <c r="C273" t="s">
-        <v>1250</v>
+        <v>1173</v>
       </c>
       <c r="D273" t="s">
-        <v>1252</v>
+        <v>1174</v>
       </c>
       <c r="E273" t="s">
-        <v>1253</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>1254</v>
+        <v>1176</v>
       </c>
       <c r="B274" t="s">
-        <v>1255</v>
+        <v>1177</v>
       </c>
       <c r="C274" t="s">
-        <v>1254</v>
+        <v>1178</v>
       </c>
       <c r="D274" t="s">
-        <v>1256</v>
+        <v>1179</v>
       </c>
       <c r="E274" t="s">
-        <v>1257</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>1258</v>
+        <v>1180</v>
       </c>
       <c r="B275" t="s">
-        <v>1259</v>
+        <v>1181</v>
       </c>
       <c r="C275" t="s">
-        <v>1258</v>
+        <v>1182</v>
       </c>
       <c r="D275" t="s">
-        <v>1260</v>
+        <v>1183</v>
       </c>
       <c r="E275" t="s">
-        <v>1261</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>1262</v>
+        <v>1185</v>
       </c>
       <c r="B276" t="s">
-        <v>1263</v>
+        <v>138</v>
       </c>
       <c r="C276" t="s">
-        <v>1262</v>
+        <v>139</v>
       </c>
       <c r="D276" t="s">
-        <v>1264</v>
+        <v>140</v>
       </c>
       <c r="E276" t="s">
-        <v>1265</v>
+        <v>140</v>
       </c>
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>569</v>
+        <v>1186</v>
       </c>
       <c r="B277" t="s">
-        <v>1266</v>
+        <v>1187</v>
       </c>
       <c r="C277" t="s">
-        <v>569</v>
+        <v>1188</v>
       </c>
       <c r="D277" t="s">
-        <v>570</v>
+        <v>1189</v>
       </c>
       <c r="E277" t="s">
-        <v>571</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
+        <v>1191</v>
+      </c>
+      <c r="B278" t="s">
+        <v>1192</v>
+      </c>
+      <c r="C278" t="s">
+        <v>1193</v>
+      </c>
+      <c r="D278" t="s">
+        <v>1194</v>
+      </c>
+      <c r="E278" t="s">
+        <v>1195</v>
+      </c>
+    </row>
+    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>1196</v>
+      </c>
+      <c r="B279" t="s">
+        <v>1197</v>
+      </c>
+      <c r="C279" t="s">
+        <v>1198</v>
+      </c>
+      <c r="D279" t="s">
+        <v>1199</v>
+      </c>
+      <c r="E279" t="s">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
+        <v>1201</v>
+      </c>
+      <c r="B280" t="s">
+        <v>1202</v>
+      </c>
+      <c r="C280" t="s">
+        <v>1203</v>
+      </c>
+      <c r="D280" t="s">
+        <v>1204</v>
+      </c>
+      <c r="E280" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
+        <v>1206</v>
+      </c>
+      <c r="B281" t="s">
+        <v>1207</v>
+      </c>
+      <c r="C281" t="s">
+        <v>1208</v>
+      </c>
+      <c r="D281" t="s">
+        <v>1209</v>
+      </c>
+      <c r="E281" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A282" t="s">
+        <v>1211</v>
+      </c>
+      <c r="B282" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C282" t="s">
+        <v>1213</v>
+      </c>
+      <c r="D282" t="s">
+        <v>1214</v>
+      </c>
+      <c r="E282" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
+        <v>1216</v>
+      </c>
+      <c r="B283" t="s">
+        <v>1217</v>
+      </c>
+      <c r="C283" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D283" t="s">
+        <v>1219</v>
+      </c>
+      <c r="E283" t="s">
+        <v>1220</v>
+      </c>
+    </row>
+    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A284" t="s">
+        <v>1221</v>
+      </c>
+      <c r="B284" t="s">
+        <v>1222</v>
+      </c>
+      <c r="C284" t="s">
+        <v>1223</v>
+      </c>
+      <c r="D284" t="s">
+        <v>1224</v>
+      </c>
+      <c r="E284" t="s">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
+        <v>1226</v>
+      </c>
+      <c r="B285" t="s">
+        <v>1227</v>
+      </c>
+      <c r="C285" t="s">
+        <v>1228</v>
+      </c>
+      <c r="D285" t="s">
+        <v>1229</v>
+      </c>
+      <c r="E285" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A286" t="s">
+        <v>1231</v>
+      </c>
+      <c r="B286" t="s">
+        <v>820</v>
+      </c>
+      <c r="C286" t="s">
+        <v>1232</v>
+      </c>
+      <c r="D286" t="s">
+        <v>1233</v>
+      </c>
+      <c r="E286" t="s">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A287" t="s">
+        <v>1235</v>
+      </c>
+      <c r="B287" t="s">
+        <v>1236</v>
+      </c>
+      <c r="C287" t="s">
+        <v>1237</v>
+      </c>
+      <c r="D287" t="s">
+        <v>1238</v>
+      </c>
+      <c r="E287" t="s">
+        <v>1239</v>
+      </c>
+    </row>
+    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B288" t="s">
+        <v>406</v>
+      </c>
+      <c r="C288" t="s">
+        <v>388</v>
+      </c>
+      <c r="D288" t="s">
+        <v>398</v>
+      </c>
+      <c r="E288" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A289" t="s">
+        <v>1241</v>
+      </c>
+      <c r="B289" t="s">
+        <v>1242</v>
+      </c>
+      <c r="C289" t="s">
+        <v>1243</v>
+      </c>
+      <c r="D289" t="s">
+        <v>1244</v>
+      </c>
+      <c r="E289" t="s">
+        <v>1245</v>
+      </c>
+    </row>
+    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A290" t="s">
+        <v>1246</v>
+      </c>
+      <c r="B290" t="s">
+        <v>123</v>
+      </c>
+      <c r="C290" t="s">
+        <v>124</v>
+      </c>
+      <c r="D290" t="s">
+        <v>616</v>
+      </c>
+      <c r="E290" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A291" t="s">
+        <v>1247</v>
+      </c>
+      <c r="B291" t="s">
+        <v>133</v>
+      </c>
+      <c r="C291" t="s">
+        <v>1248</v>
+      </c>
+      <c r="D291" t="s">
+        <v>1249</v>
+      </c>
+      <c r="E291" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A292" t="s">
+        <v>1250</v>
+      </c>
+      <c r="B292" t="s">
+        <v>128</v>
+      </c>
+      <c r="C292" t="s">
+        <v>129</v>
+      </c>
+      <c r="D292" t="s">
+        <v>1251</v>
+      </c>
+      <c r="E292" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A293" t="s">
+        <v>1252</v>
+      </c>
+      <c r="B293" t="s">
+        <v>138</v>
+      </c>
+      <c r="C293" t="s">
+        <v>139</v>
+      </c>
+      <c r="D293" t="s">
+        <v>140</v>
+      </c>
+      <c r="E293" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A294" t="s">
+        <v>1253</v>
+      </c>
+      <c r="B294" t="s">
+        <v>1254</v>
+      </c>
+      <c r="C294" t="s">
+        <v>1255</v>
+      </c>
+      <c r="D294" t="s">
+        <v>1256</v>
+      </c>
+      <c r="E294" t="s">
+        <v>1257</v>
+      </c>
+    </row>
+    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A295" t="s">
+        <v>1258</v>
+      </c>
+      <c r="B295" t="s">
+        <v>492</v>
+      </c>
+      <c r="C295" t="s">
+        <v>493</v>
+      </c>
+      <c r="D295" t="s">
+        <v>494</v>
+      </c>
+      <c r="E295" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A296" t="s">
+        <v>1259</v>
+      </c>
+      <c r="B296" t="s">
+        <v>1260</v>
+      </c>
+      <c r="C296" t="s">
+        <v>1261</v>
+      </c>
+      <c r="D296" t="s">
+        <v>1262</v>
+      </c>
+      <c r="E296" t="s">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A297" t="s">
+        <v>1264</v>
+      </c>
+      <c r="B297" t="s">
+        <v>1265</v>
+      </c>
+      <c r="C297" t="s">
+        <v>1266</v>
+      </c>
+      <c r="D297" t="s">
+        <v>1267</v>
+      </c>
+      <c r="E297" t="s">
+        <v>1268</v>
+      </c>
+    </row>
+    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A298" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B298" t="s">
+        <v>16</v>
+      </c>
+      <c r="C298" t="s">
+        <v>1270</v>
+      </c>
+      <c r="D298" t="s">
+        <v>18</v>
+      </c>
+      <c r="E298" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A299" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B299" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C299" t="s">
+        <v>1272</v>
+      </c>
+      <c r="D299" t="s">
+        <v>1273</v>
+      </c>
+      <c r="E299" t="s">
+        <v>1274</v>
+      </c>
+    </row>
+    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A300" t="s">
+        <v>1275</v>
+      </c>
+      <c r="B300" t="s">
+        <v>1275</v>
+      </c>
+      <c r="C300" t="s">
+        <v>1276</v>
+      </c>
+      <c r="D300" t="s">
+        <v>1277</v>
+      </c>
+      <c r="E300" t="s">
+        <v>1277</v>
+      </c>
+    </row>
+    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A301" t="s">
+        <v>1278</v>
+      </c>
+      <c r="B301" t="s">
+        <v>1278</v>
+      </c>
+      <c r="C301" t="s">
+        <v>1279</v>
+      </c>
+      <c r="D301" t="s">
+        <v>1280</v>
+      </c>
+      <c r="E301" t="s">
+        <v>1281</v>
+      </c>
+    </row>
+    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A302" t="s">
+        <v>1282</v>
+      </c>
+      <c r="B302" t="s">
+        <v>1282</v>
+      </c>
+      <c r="C302" t="s">
+        <v>1283</v>
+      </c>
+      <c r="D302" t="s">
+        <v>1284</v>
+      </c>
+      <c r="E302" t="s">
+        <v>1284</v>
+      </c>
+    </row>
+    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A303" t="s">
+        <v>1285</v>
+      </c>
+      <c r="B303" t="s">
+        <v>1285</v>
+      </c>
+      <c r="C303" t="s">
+        <v>1286</v>
+      </c>
+      <c r="D303" t="s">
+        <v>1287</v>
+      </c>
+      <c r="E303" t="s">
+        <v>1288</v>
+      </c>
+    </row>
+    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A304" t="s">
+        <v>133</v>
+      </c>
+      <c r="B304" t="s">
+        <v>133</v>
+      </c>
+      <c r="C304" t="s">
+        <v>134</v>
+      </c>
+      <c r="D304" t="s">
+        <v>1249</v>
+      </c>
+      <c r="E304" t="s">
+        <v>1289</v>
+      </c>
+    </row>
+    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A305" t="s">
+        <v>1290</v>
+      </c>
+      <c r="B305" t="s">
+        <v>1290</v>
+      </c>
+      <c r="C305" t="s">
+        <v>1291</v>
+      </c>
+      <c r="D305" t="s">
+        <v>1292</v>
+      </c>
+      <c r="E305" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A306" t="s">
+        <v>1293</v>
+      </c>
+      <c r="B306" t="s">
+        <v>1293</v>
+      </c>
+      <c r="C306" t="s">
+        <v>1294</v>
+      </c>
+      <c r="D306" t="s">
+        <v>1295</v>
+      </c>
+      <c r="E306" t="s">
+        <v>1296</v>
+      </c>
+    </row>
+    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A307" t="s">
+        <v>1297</v>
+      </c>
+      <c r="B307" t="s">
+        <v>1207</v>
+      </c>
+      <c r="C307" t="s">
+        <v>1208</v>
+      </c>
+      <c r="D307" t="s">
+        <v>1298</v>
+      </c>
+      <c r="E307" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A308" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B308" t="s">
+        <v>1299</v>
+      </c>
+      <c r="C308" t="s">
+        <v>1300</v>
+      </c>
+      <c r="D308" t="s">
+        <v>1301</v>
+      </c>
+      <c r="E308" t="s">
+        <v>1302</v>
+      </c>
+    </row>
+    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A309" t="s">
+        <v>1303</v>
+      </c>
+      <c r="B309" t="s">
+        <v>1303</v>
+      </c>
+      <c r="C309" t="s">
+        <v>1304</v>
+      </c>
+      <c r="D309" t="s">
+        <v>1305</v>
+      </c>
+      <c r="E309" t="s">
+        <v>1306</v>
+      </c>
+    </row>
+    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A310" t="s">
+        <v>1307</v>
+      </c>
+      <c r="B310" t="s">
+        <v>1307</v>
+      </c>
+      <c r="C310" t="s">
+        <v>1308</v>
+      </c>
+      <c r="D310" t="s">
+        <v>1309</v>
+      </c>
+      <c r="E310" t="s">
+        <v>1310</v>
+      </c>
+    </row>
+    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A311" t="s">
+        <v>1311</v>
+      </c>
+      <c r="B311" t="s">
+        <v>1311</v>
+      </c>
+      <c r="C311" t="s">
+        <v>1312</v>
+      </c>
+      <c r="D311" t="s">
+        <v>1313</v>
+      </c>
+      <c r="E311" t="s">
+        <v>1314</v>
+      </c>
+    </row>
+    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A312" t="s">
+        <v>1315</v>
+      </c>
+      <c r="B312" t="s">
+        <v>1316</v>
+      </c>
+      <c r="C312" t="s">
+        <v>1317</v>
+      </c>
+      <c r="D312" t="s">
+        <v>1318</v>
+      </c>
+      <c r="E312" t="s">
+        <v>1319</v>
+      </c>
+    </row>
+    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A313" t="s">
+        <v>1320</v>
+      </c>
+      <c r="B313" t="s">
+        <v>1321</v>
+      </c>
+      <c r="C313" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D313" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E313" t="s">
+        <v>1324</v>
+      </c>
+    </row>
+    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A314" t="s">
+        <v>1325</v>
+      </c>
+      <c r="B314" t="s">
+        <v>1326</v>
+      </c>
+      <c r="C314" t="s">
+        <v>1327</v>
+      </c>
+      <c r="D314" t="s">
+        <v>1328</v>
+      </c>
+      <c r="E314" t="s">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A315" t="s">
+        <v>1330</v>
+      </c>
+      <c r="B315" t="s">
+        <v>1331</v>
+      </c>
+      <c r="C315" t="s">
+        <v>1332</v>
+      </c>
+      <c r="D315" t="s">
+        <v>1333</v>
+      </c>
+      <c r="E315" t="s">
+        <v>1334</v>
+      </c>
+    </row>
+    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A316" t="s">
+        <v>1335</v>
+      </c>
+      <c r="B316" t="s">
+        <v>1336</v>
+      </c>
+      <c r="C316" t="s">
+        <v>1337</v>
+      </c>
+      <c r="D316" t="s">
+        <v>1338</v>
+      </c>
+      <c r="E316" t="s">
+        <v>1339</v>
+      </c>
+    </row>
+    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A317" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B317" t="s">
+        <v>1341</v>
+      </c>
+      <c r="C317" t="s">
+        <v>1340</v>
+      </c>
+      <c r="D317" t="s">
+        <v>1342</v>
+      </c>
+      <c r="E317" t="s">
+        <v>1343</v>
+      </c>
+    </row>
+    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A318" t="s">
+        <v>1344</v>
+      </c>
+      <c r="B318" t="s">
+        <v>1345</v>
+      </c>
+      <c r="C318" t="s">
+        <v>1344</v>
+      </c>
+      <c r="D318" t="s">
+        <v>1346</v>
+      </c>
+      <c r="E318" t="s">
+        <v>1347</v>
+      </c>
+    </row>
+    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A319" t="s">
+        <v>1348</v>
+      </c>
+      <c r="B319" t="s">
+        <v>1349</v>
+      </c>
+      <c r="C319" t="s">
+        <v>1348</v>
+      </c>
+      <c r="D319" t="s">
+        <v>1350</v>
+      </c>
+      <c r="E319" t="s">
+        <v>1351</v>
+      </c>
+    </row>
+    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A320" t="s">
+        <v>1352</v>
+      </c>
+      <c r="B320" t="s">
+        <v>1353</v>
+      </c>
+      <c r="C320" t="s">
+        <v>1352</v>
+      </c>
+      <c r="D320" t="s">
+        <v>1354</v>
+      </c>
+      <c r="E320" t="s">
+        <v>1355</v>
+      </c>
+    </row>
+    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A321" t="s">
+        <v>569</v>
+      </c>
+      <c r="B321" t="s">
+        <v>609</v>
+      </c>
+      <c r="C321" t="s">
+        <v>569</v>
+      </c>
+      <c r="D321" t="s">
+        <v>570</v>
+      </c>
+      <c r="E321" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="322" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A322" t="s">
         <v>593</v>
       </c>
-      <c r="B278" t="s">
-        <v>1266</v>
-      </c>
-      <c r="C278" t="s">
+      <c r="B322" t="s">
+        <v>609</v>
+      </c>
+      <c r="C322" t="s">
         <v>593</v>
       </c>
-      <c r="D278" t="s">
+      <c r="D322" t="s">
         <v>594</v>
       </c>
-      <c r="E278" t="s">
+      <c r="E322" t="s">
         <v>595</v>
+      </c>
+    </row>
+    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A323" t="s">
+        <v>1356</v>
+      </c>
+      <c r="B323" t="s">
+        <v>1356</v>
+      </c>
+      <c r="C323" t="s">
+        <v>1357</v>
+      </c>
+      <c r="D323" t="s">
+        <v>1358</v>
+      </c>
+      <c r="E323" t="s">
+        <v>1359</v>
+      </c>
+    </row>
+    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A324" t="s">
+        <v>1360</v>
+      </c>
+      <c r="B324" t="s">
+        <v>1361</v>
+      </c>
+      <c r="C324" t="s">
+        <v>1361</v>
+      </c>
+      <c r="D324" t="s">
+        <v>1362</v>
+      </c>
+      <c r="E324" t="s">
+        <v>1362</v>
+      </c>
+    </row>
+    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A325" t="s">
+        <v>1363</v>
+      </c>
+      <c r="B325" t="s">
+        <v>1364</v>
+      </c>
+      <c r="C325" t="s">
+        <v>1365</v>
+      </c>
+      <c r="D325" t="s">
+        <v>1366</v>
+      </c>
+      <c r="E325" t="s">
+        <v>1367</v>
+      </c>
+    </row>
+    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A326" t="s">
+        <v>1368</v>
+      </c>
+      <c r="B326" t="s">
+        <v>1369</v>
+      </c>
+      <c r="C326" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D326" t="s">
+        <v>1371</v>
+      </c>
+      <c r="E326" t="s">
+        <v>1372</v>
+      </c>
+    </row>
+    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A327" t="s">
+        <v>1373</v>
+      </c>
+      <c r="B327" t="s">
+        <v>1374</v>
+      </c>
+      <c r="C327" t="s">
+        <v>1375</v>
+      </c>
+      <c r="D327" t="s">
+        <v>1376</v>
+      </c>
+      <c r="E327" t="s">
+        <v>1377</v>
       </c>
     </row>
   </sheetData>

</xml_diff>